<commit_message>
eddited the availableProjects with the projects I choose.
</commit_message>
<xml_diff>
--- a/availableProjects.xlsx
+++ b/availableProjects.xlsx
@@ -179,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -202,15 +202,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -529,19 +556,19 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -549,7 +576,9 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -563,13 +592,15 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G38" si="0">SUM(B3:F3)</f>
+        <f t="shared" ref="G3:G39" si="0">SUM(B3:F3)</f>
         <v>0</v>
       </c>
     </row>
@@ -577,7 +608,9 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -591,7 +624,9 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -605,7 +640,9 @@
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -619,7 +656,9 @@
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -633,7 +672,9 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -647,7 +688,9 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -661,7 +704,9 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -675,7 +720,9 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -689,7 +736,9 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -703,7 +752,9 @@
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -717,7 +768,9 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -731,7 +784,9 @@
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -745,7 +800,9 @@
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -759,7 +816,9 @@
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -773,7 +832,9 @@
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -787,7 +848,9 @@
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -801,7 +864,9 @@
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -815,7 +880,9 @@
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -829,7 +896,9 @@
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -843,7 +912,9 @@
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -857,7 +928,9 @@
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -871,21 +944,25 @@
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -899,7 +976,9 @@
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -913,7 +992,9 @@
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -927,21 +1008,25 @@
       <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -955,7 +1040,9 @@
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -969,7 +1056,9 @@
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -983,7 +1072,9 @@
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -997,21 +1088,25 @@
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1025,7 +1120,9 @@
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1039,7 +1136,9 @@
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1050,18 +1149,29 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B38" s="7">
+        <v>0</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Semaka: added my choices
</commit_message>
<xml_diff>
--- a/availableProjects.xlsx
+++ b/availableProjects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lana\Documents\UP\COS 301\Main Project\GIT\MainProjectCOS301\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Residences\MainProjectCOS301\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,9 +588,7 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -604,9 +602,7 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -620,25 +616,23 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -652,9 +646,7 @@
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -668,9 +660,7 @@
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -684,9 +674,7 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -700,9 +688,7 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -716,9 +702,7 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -732,9 +716,7 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -748,9 +730,7 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -764,9 +744,7 @@
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -780,27 +758,25 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
       <c r="F14" s="2">
         <v>1</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -814,9 +790,7 @@
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -830,9 +804,7 @@
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -846,9 +818,7 @@
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -862,9 +832,7 @@
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -878,9 +846,7 @@
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -894,9 +860,7 @@
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -910,9 +874,7 @@
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -926,9 +888,7 @@
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -942,9 +902,7 @@
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -978,9 +936,7 @@
       <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -994,9 +950,7 @@
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="2">
-        <v>0</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1010,9 +964,7 @@
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1048,9 +1000,7 @@
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="2">
-        <v>0</v>
-      </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1064,9 +1014,7 @@
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="2">
-        <v>0</v>
-      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1080,9 +1028,7 @@
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
-      </c>
+      <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2">
         <v>1</v>
@@ -1114,9 +1060,7 @@
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2">
-        <v>0</v>
-      </c>
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1130,29 +1074,27 @@
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="2">
-        <v>0</v>
-      </c>
+      <c r="B35" s="2"/>
       <c r="C35" s="2">
         <v>1</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="2">
-        <v>0</v>
-      </c>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1166,9 +1108,7 @@
       <c r="A37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="7">
-        <v>0</v>
-      </c>
+      <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>

</xml_diff>

<commit_message>
highlited winning choises for tenders
</commit_message>
<xml_diff>
--- a/availableProjects.xlsx
+++ b/availableProjects.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Residences\MainProjectCOS301\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="7500"/>
   </bookViews>
@@ -155,8 +150,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,12 +168,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -230,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -240,6 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,7 +302,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,10 +334,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,7 +368,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -543,14 +543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="63.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -561,7 +561,7 @@
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -598,7 +598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -628,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -656,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -726,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -754,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -772,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -898,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -912,27 +912,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9">
+        <v>1</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
@@ -946,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -974,29 +974,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2">
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
@@ -1070,27 +1070,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="6" t="s">
         <v>42</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="5"/>
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
@@ -1134,24 +1134,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>